<commit_message>
Make DrawingVisual perform equal to DrawingContext
</commit_message>
<xml_diff>
--- a/Drawing Performance Comparisons.xlsx
+++ b/Drawing Performance Comparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\WpfDrawingOptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E19D75-E4DB-43DF-AFD4-5CEEFA2B9DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33807CE8-EF7A-49BF-A39E-10F5AB60D1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{563D8AC9-4C7D-4D50-B9DD-B1DB98568A2D}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{563D8AC9-4C7D-4D50-B9DD-B1DB98568A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>Technology</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>Immediate</t>
   </si>
   <si>
     <t>Compositable?</t>
@@ -585,7 +582,7 @@
   <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +622,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>2</v>
@@ -681,7 +678,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" s="2">
         <v>25000</v>
@@ -710,7 +707,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" s="2">
         <v>25000</v>
@@ -739,7 +736,7 @@
         <v>29</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" s="2"/>
       <c r="M4" s="2"/>
@@ -754,13 +751,13 @@
         <v>5000</v>
       </c>
       <c r="F5" s="4">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G5" s="4">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="2">
         <v>25000</v>
@@ -776,9 +773,6 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
-        <v>32</v>
-      </c>
       <c r="C6" s="10" t="s">
         <v>31</v>
       </c>
@@ -789,13 +783,13 @@
         <v>5000</v>
       </c>
       <c r="F6" s="4">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G6" s="4">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" s="2">
         <v>25000</v>
@@ -818,13 +812,13 @@
         <v>5000</v>
       </c>
       <c r="F7" s="4">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G7" s="4">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" s="2">
         <v>25000</v>
@@ -853,7 +847,7 @@
         <v>0.2</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I8" s="2">
         <v>25000</v>
@@ -882,7 +876,7 @@
         <v>20</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I9" s="2"/>
       <c r="M9" s="2"/>
@@ -912,7 +906,7 @@
         <v>60</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I10" s="3">
         <v>25000</v>
@@ -977,7 +971,7 @@
         <v>60</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11" s="8">
         <v>25000</v>
@@ -1042,7 +1036,7 @@
         <v>60</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I12" s="3">
         <v>25000</v>
@@ -1107,7 +1101,7 @@
         <v>30</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I13" s="8">
         <v>25000</v>
@@ -1172,7 +1166,7 @@
         <v>45</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I14" s="3">
         <v>25000</v>

</xml_diff>